<commit_message>
currency filtering and ensure property tiles currency changed: Done(Only checked for USD currency)
</commit_message>
<xml_diff>
--- a/test_report.xlsx
+++ b/test_report.xlsx
@@ -2,29 +2,34 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Report" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="URL Status" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Currency Change Test" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -50,12 +55,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -424,7 +430,14 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <cols>
+    <col width="71.1796875" customWidth="1" min="1" max="1"/>
+    <col width="22.08984375" customWidth="1" min="2" max="2"/>
+    <col width="8.08984375" customWidth="1" min="3" max="3"/>
+    <col width="33.6328125" customWidth="1" min="4" max="4"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -483,12 +496,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sequence broken: [1, 3, 2, 3, 3, 3, 3, 3, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 3, 2, 2, 2, 2, 2, 2, 2, 2, 3, 2, 3, 4]</t>
+          <t>Sequence correct: [1, 2]</t>
         </is>
       </c>
     </row>
@@ -527,12 +540,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2 broken links found</t>
+          <t>No broken links found</t>
         </is>
       </c>
     </row>
@@ -547,7 +560,43 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,53 +605,574 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>URL</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Comments</t>
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Card Number</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Initial Price</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Updated Price</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Test Result</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/StaysTravel</t>
+          <t>Card 1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>De €169</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Request error: HTTPSConnectionPool(host='www.facebook.com', port=443): Max retries exceeded with url: /StaysTravel (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x720ac9fbaed0&gt;: Failed to resolve 'www.facebook.com' ([Errno -3] Temporary failure in name resolution)"))</t>
+          <t>De $177</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/StaysTravel</t>
+          <t>Card 2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>De €576</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Request error: HTTPSConnectionPool(host='www.facebook.com', port=443): Max retries exceeded with url: /StaysTravel (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x720ac9fbb740&gt;: Failed to resolve 'www.facebook.com' ([Errno -3] Temporary failure in name resolution)"))</t>
+          <t>De $605</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Card 3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>De €299</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>De $314</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Card 4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>De €168</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>De $176</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Card 5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>De €2,343</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>De $2,459</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Card 6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>De €207</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>De $217</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Card 7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>De €183</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>De $192</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Card 8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>De €80</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>De $84</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Card 9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>De €286</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>De $300</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Card 10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>De €153</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>De $161</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Card 11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>De €109</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>De $115</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Card 12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>De €511</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>De $536</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Card 13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>De €111</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>De $116</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Card 14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>De €413</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>De $433</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Card 15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>De €372</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>De $390</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Card 16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>De €255</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>De $268</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Card 17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>De €221</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>De $232</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Card 18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>De €752</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>De $789</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Card 19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>De €251</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>De $263</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Card 20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>De €1,454</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>De $1,526</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Card 21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>De €68</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>De $72</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Card 22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>De €36</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>De $38</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Card 23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>De €227</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>De $238</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Card 24</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>De €245</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>De $257</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Availability Price Test</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>EUR €169</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>USD $177</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>PASS (Currency changed successfully)</t>
         </is>
       </c>
     </row>

</xml_diff>